<commit_message>
add the water transfer file HB compiled
</commit_message>
<xml_diff>
--- a/maxs_work/bulletin_132_work/transfers_by_buyer_new.xlsx
+++ b/maxs_work/bulletin_132_work/transfers_by_buyer_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxslesinski/Documents/GitHub/dlkency_CALFEWS/CALFEWS/maxs_work/bulletin_132_work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/danli_ad_unc_edu/Documents/github/CALFEWS/maxs_work/bulletin_132_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F65D17-A1D1-3141-B8F3-140EC276AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A8F65D17-A1D1-3141-B8F3-140EC276AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C1FE230-8F4C-4633-9F7A-6E7E74BCE4B0}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="500" windowWidth="13740" windowHeight="16280" xr2:uid="{CAEF76C3-CC13-994B-AF76-6F3F7E947AA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="592" xr2:uid="{CAEF76C3-CC13-994B-AF76-6F3F7E947AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,15 +535,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF4683E-4F28-3349-940D-48DD80CE5C9C}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -587,7 +593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -604,7 +610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -621,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -638,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -655,7 +661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -672,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -689,7 +695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -706,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -723,7 +729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -740,7 +746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -757,7 +763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -774,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -791,7 +797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -808,7 +814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -825,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -842,7 +848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -859,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -876,7 +882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -893,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -910,7 +916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -927,7 +933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -944,7 +950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -961,7 +967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -978,7 +984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1080,105 +1086,105 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>14650</v>
       </c>
-      <c r="E32" s="2">
-        <v>2021</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="E32">
+        <v>2021</v>
+      </c>
+      <c r="F32" t="s">
         <v>36</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>500</v>
       </c>
-      <c r="E33" s="2">
-        <v>2021</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="E33">
+        <v>2021</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>5000</v>
       </c>
-      <c r="E34" s="2">
-        <v>2021</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="E34">
+        <v>2021</v>
+      </c>
+      <c r="F34" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>5500</v>
       </c>
-      <c r="E35" s="2">
-        <v>2021</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>2021</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>2000</v>
       </c>
-      <c r="E36" s="2">
-        <v>2021</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>2021</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>76069</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>2021</v>
       </c>
       <c r="F37" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>